<commit_message>
Preliminary officer corps work
</commit_message>
<xml_diff>
--- a/Modding resources/Generals rework/general_skils.xlsx
+++ b/Modding resources/Generals rework/general_skils.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Niko\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Niko\Documents\Paradox Interactive\Hearts of Iron IV\mod\Millennium_Dawn\Modding resources\Generals rework\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2029189-4C5E-4F27-81A5-64C3EC739A98}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6E32A34-F981-45DA-AFCA-D7922459285B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{511A6305-1776-4F22-95A5-78D4235C4494}"/>
   </bookViews>
@@ -249,14 +249,14 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
       <xdr:colOff>1323975</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:rowOff>9525</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -271,7 +271,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="609600" y="1790700"/>
+          <a:off x="609600" y="1781175"/>
           <a:ext cx="2628900" cy="781050"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1294,7 +1294,7 @@
       <xdr:col>2</xdr:col>
       <xdr:colOff>1323975</xdr:colOff>
       <xdr:row>11</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
@@ -1318,8 +1318,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3238500" y="2181225"/>
-          <a:ext cx="266700" cy="19050"/>
+          <a:off x="3238500" y="2171700"/>
+          <a:ext cx="266700" cy="28575"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -1634,7 +1634,7 @@
       <xdr:col>2</xdr:col>
       <xdr:colOff>1323975</xdr:colOff>
       <xdr:row>11</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
@@ -1658,8 +1658,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3238500" y="2181225"/>
-          <a:ext cx="266700" cy="952500"/>
+          <a:off x="3238500" y="2171700"/>
+          <a:ext cx="266700" cy="962025"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector3">
           <a:avLst>
@@ -9590,8 +9590,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7BA517C-D1A9-4F75-96FE-45E960B0DE9C}">
   <dimension ref="B3:O16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Army leader starting traits
</commit_message>
<xml_diff>
--- a/Modding resources/Generals rework/general_skils.xlsx
+++ b/Modding resources/Generals rework/general_skils.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Niko\Documents\Paradox Interactive\Hearts of Iron IV\mod\Millennium_Dawn\Modding resources\Generals rework\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6E32A34-F981-45DA-AFCA-D7922459285B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2699C333-0D8D-46FD-9481-F74F1337A555}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{511A6305-1776-4F22-95A5-78D4235C4494}"/>
   </bookViews>
@@ -1689,14 +1689,14 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>600075</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>19</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>1314450</xdr:colOff>
+      <xdr:colOff>1323975</xdr:colOff>
       <xdr:row>23</xdr:row>
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:to>
@@ -1713,7 +1713,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="600075" y="3695700"/>
+          <a:off x="609600" y="3695700"/>
           <a:ext cx="2628900" cy="781050"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1976,7 +1976,7 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>1314450</xdr:colOff>
+      <xdr:colOff>1323975</xdr:colOff>
       <xdr:row>21</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
@@ -2002,8 +2002,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3228975" y="4086225"/>
-          <a:ext cx="276225" cy="0"/>
+          <a:off x="3238500" y="4086225"/>
+          <a:ext cx="266700" cy="0"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -2265,7 +2265,7 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>1314450</xdr:colOff>
+      <xdr:colOff>1323975</xdr:colOff>
       <xdr:row>16</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
@@ -2291,8 +2291,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="3228975" y="3133725"/>
-          <a:ext cx="276225" cy="952500"/>
+          <a:off x="3238500" y="3133725"/>
+          <a:ext cx="266700" cy="952500"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector3">
           <a:avLst>
@@ -9590,8 +9590,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7BA517C-D1A9-4F75-96FE-45E960B0DE9C}">
   <dimension ref="B3:O16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
New army leader trait setup
</commit_message>
<xml_diff>
--- a/Modding resources/Generals rework/general_skils.xlsx
+++ b/Modding resources/Generals rework/general_skils.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Niko\Documents\Paradox Interactive\Hearts of Iron IV\mod\Millennium_Dawn\Modding resources\Generals rework\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2699C333-0D8D-46FD-9481-F74F1337A555}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4D01CF4-4D88-4FE2-95ED-2A1178548145}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{511A6305-1776-4F22-95A5-78D4235C4494}"/>
   </bookViews>
@@ -9590,8 +9590,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7BA517C-D1A9-4F75-96FE-45E960B0DE9C}">
   <dimension ref="B3:O16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J31" sqref="J31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>